<commit_message>
Removed filters from excel database
</commit_message>
<xml_diff>
--- a/data/NutrientMgmt_AgEvidence.xlsx
+++ b/data/NutrientMgmt_AgEvidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LWA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LWA\Documents\Github\AgEvidence-master\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE1F22B8-45D7-4A31-8F6C-75E43C164360}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0C99D5-DFE2-4FA7-9F06-7762560485DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18970" windowHeight="5220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="13" r:id="rId1"/>
@@ -6185,9 +6185,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:AO1048576"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -11039,7 +11039,6 @@
       <c r="A1000" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{0DF2EDAD-9114-412F-8122-3C3F59DCF98C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -11047,12 +11046,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA711F7-0F73-440F-8A53-7FEBBD1E9456}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H87" sqref="H87"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11140,7 +11138,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="2" spans="1:26" hidden="1">
+    <row r="2" spans="1:26">
       <c r="A2" s="66">
         <v>120</v>
       </c>
@@ -11220,7 +11218,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="3" spans="1:26" hidden="1">
+    <row r="3" spans="1:26">
       <c r="A3" s="66">
         <v>120</v>
       </c>
@@ -11300,7 +11298,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="4" spans="1:26" hidden="1">
+    <row r="4" spans="1:26">
       <c r="A4" s="66">
         <v>120</v>
       </c>
@@ -11380,7 +11378,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="5" spans="1:26" hidden="1">
+    <row r="5" spans="1:26">
       <c r="A5" s="66">
         <v>121</v>
       </c>
@@ -11460,7 +11458,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="6" spans="1:26" hidden="1">
+    <row r="6" spans="1:26">
       <c r="A6" s="66">
         <v>121</v>
       </c>
@@ -11540,7 +11538,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="7" spans="1:26" hidden="1">
+    <row r="7" spans="1:26">
       <c r="A7" s="66">
         <v>121</v>
       </c>
@@ -11620,7 +11618,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="8" spans="1:26" hidden="1">
+    <row r="8" spans="1:26">
       <c r="A8" s="66">
         <v>121</v>
       </c>
@@ -11700,7 +11698,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="9" spans="1:26" hidden="1">
+    <row r="9" spans="1:26">
       <c r="A9" s="66">
         <v>121</v>
       </c>
@@ -11780,7 +11778,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="10" spans="1:26" hidden="1">
+    <row r="10" spans="1:26">
       <c r="A10" s="66">
         <v>121</v>
       </c>
@@ -11860,7 +11858,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="11" spans="1:26" hidden="1">
+    <row r="11" spans="1:26">
       <c r="A11" s="66">
         <v>122</v>
       </c>
@@ -11940,7 +11938,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="12" spans="1:26" hidden="1">
+    <row r="12" spans="1:26">
       <c r="A12" s="66">
         <v>123</v>
       </c>
@@ -12020,7 +12018,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="13" spans="1:26" hidden="1">
+    <row r="13" spans="1:26">
       <c r="A13" s="66">
         <v>123</v>
       </c>
@@ -12100,7 +12098,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="14" spans="1:26" hidden="1">
+    <row r="14" spans="1:26">
       <c r="A14" s="66">
         <v>123</v>
       </c>
@@ -12180,7 +12178,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="15" spans="1:26" hidden="1">
+    <row r="15" spans="1:26">
       <c r="A15" s="66">
         <v>123</v>
       </c>
@@ -12260,7 +12258,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="16" spans="1:26" hidden="1">
+    <row r="16" spans="1:26">
       <c r="A16" s="66">
         <v>124</v>
       </c>
@@ -12340,7 +12338,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="17" spans="1:26" hidden="1">
+    <row r="17" spans="1:26">
       <c r="A17" s="66">
         <v>124</v>
       </c>
@@ -12420,7 +12418,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="18" spans="1:26" hidden="1">
+    <row r="18" spans="1:26">
       <c r="A18" s="66">
         <v>125</v>
       </c>
@@ -12500,7 +12498,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="19" spans="1:26" hidden="1">
+    <row r="19" spans="1:26">
       <c r="A19" s="66">
         <v>126</v>
       </c>
@@ -12580,7 +12578,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="20" spans="1:26" hidden="1">
+    <row r="20" spans="1:26">
       <c r="A20" s="66">
         <v>126</v>
       </c>
@@ -12660,7 +12658,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="21" spans="1:26" hidden="1">
+    <row r="21" spans="1:26">
       <c r="A21" s="66">
         <v>126</v>
       </c>
@@ -12740,7 +12738,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="22" spans="1:26" hidden="1">
+    <row r="22" spans="1:26">
       <c r="A22" s="66">
         <v>126</v>
       </c>
@@ -12820,7 +12818,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="23" spans="1:26" hidden="1">
+    <row r="23" spans="1:26">
       <c r="A23" s="66">
         <v>126</v>
       </c>
@@ -12900,7 +12898,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="24" spans="1:26" hidden="1">
+    <row r="24" spans="1:26">
       <c r="A24" s="66">
         <v>127</v>
       </c>
@@ -12980,7 +12978,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="25" spans="1:26" hidden="1">
+    <row r="25" spans="1:26">
       <c r="A25" s="66">
         <v>128</v>
       </c>
@@ -13060,7 +13058,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="26" spans="1:26" hidden="1">
+    <row r="26" spans="1:26">
       <c r="A26" s="66">
         <v>129</v>
       </c>
@@ -13140,7 +13138,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="27" spans="1:26" hidden="1">
+    <row r="27" spans="1:26">
       <c r="A27" s="66">
         <v>130</v>
       </c>
@@ -13220,7 +13218,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="28" spans="1:26" hidden="1">
+    <row r="28" spans="1:26">
       <c r="A28" s="66">
         <v>131</v>
       </c>
@@ -13300,7 +13298,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="29" spans="1:26" hidden="1">
+    <row r="29" spans="1:26">
       <c r="A29" s="66">
         <v>131</v>
       </c>
@@ -13380,7 +13378,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="30" spans="1:26" hidden="1">
+    <row r="30" spans="1:26">
       <c r="A30" s="66">
         <v>131</v>
       </c>
@@ -13460,7 +13458,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="31" spans="1:26" hidden="1">
+    <row r="31" spans="1:26">
       <c r="A31" s="66">
         <v>131</v>
       </c>
@@ -13540,7 +13538,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="32" spans="1:26" hidden="1">
+    <row r="32" spans="1:26">
       <c r="A32" s="66">
         <v>131</v>
       </c>
@@ -13620,7 +13618,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
+    <row r="33" spans="1:26">
       <c r="A33" s="66">
         <v>131</v>
       </c>
@@ -13700,7 +13698,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
+    <row r="34" spans="1:26">
       <c r="A34" s="66">
         <v>132</v>
       </c>
@@ -13780,7 +13778,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
+    <row r="35" spans="1:26">
       <c r="A35" s="66">
         <v>133</v>
       </c>
@@ -13860,7 +13858,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
+    <row r="36" spans="1:26">
       <c r="A36" s="66">
         <v>133</v>
       </c>
@@ -13940,7 +13938,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
+    <row r="37" spans="1:26">
       <c r="A37" s="66">
         <v>133</v>
       </c>
@@ -14020,7 +14018,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="38" spans="1:26" hidden="1">
+    <row r="38" spans="1:26">
       <c r="A38" s="66">
         <v>133</v>
       </c>
@@ -14100,7 +14098,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
+    <row r="39" spans="1:26">
       <c r="A39" s="66">
         <v>134</v>
       </c>
@@ -14180,7 +14178,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
+    <row r="40" spans="1:26">
       <c r="A40" s="66">
         <v>134</v>
       </c>
@@ -14260,7 +14258,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
+    <row r="41" spans="1:26">
       <c r="A41" s="66">
         <v>134</v>
       </c>
@@ -14340,7 +14338,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
+    <row r="42" spans="1:26">
       <c r="A42" s="66">
         <v>134</v>
       </c>
@@ -14420,7 +14418,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
+    <row r="43" spans="1:26">
       <c r="A43" s="66">
         <v>134</v>
       </c>
@@ -14500,7 +14498,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
+    <row r="44" spans="1:26">
       <c r="A44" s="66">
         <v>134</v>
       </c>
@@ -14580,7 +14578,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
+    <row r="45" spans="1:26">
       <c r="A45" s="66">
         <v>135</v>
       </c>
@@ -14660,7 +14658,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
+    <row r="46" spans="1:26">
       <c r="A46" s="66">
         <v>135</v>
       </c>
@@ -14740,7 +14738,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
+    <row r="47" spans="1:26">
       <c r="A47" s="66">
         <v>136</v>
       </c>
@@ -14820,7 +14818,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
+    <row r="48" spans="1:26">
       <c r="A48" s="66">
         <v>137</v>
       </c>
@@ -14900,7 +14898,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="49" spans="1:26" hidden="1">
+    <row r="49" spans="1:26">
       <c r="A49" s="66">
         <v>138</v>
       </c>
@@ -14980,7 +14978,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="50" spans="1:26" hidden="1">
+    <row r="50" spans="1:26">
       <c r="A50" s="66">
         <v>138</v>
       </c>
@@ -15140,7 +15138,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="52" spans="1:26" hidden="1">
+    <row r="52" spans="1:26">
       <c r="A52" s="66">
         <v>140</v>
       </c>
@@ -15220,7 +15218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:26" hidden="1">
+    <row r="53" spans="1:26">
       <c r="A53" s="66">
         <v>140</v>
       </c>
@@ -15300,7 +15298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:26" hidden="1">
+    <row r="54" spans="1:26">
       <c r="A54" s="66">
         <v>141</v>
       </c>
@@ -15380,7 +15378,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="55" spans="1:26" hidden="1">
+    <row r="55" spans="1:26">
       <c r="A55" s="66">
         <v>141</v>
       </c>
@@ -15460,7 +15458,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="56" spans="1:26" hidden="1">
+    <row r="56" spans="1:26">
       <c r="A56" s="66">
         <v>142</v>
       </c>
@@ -15540,7 +15538,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="57" spans="1:26" hidden="1">
+    <row r="57" spans="1:26">
       <c r="A57" s="66">
         <v>142</v>
       </c>
@@ -15620,7 +15618,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="58" spans="1:26" hidden="1">
+    <row r="58" spans="1:26">
       <c r="A58" s="66">
         <v>143</v>
       </c>
@@ -15700,7 +15698,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="59" spans="1:26" hidden="1">
+    <row r="59" spans="1:26">
       <c r="A59" s="66">
         <v>143</v>
       </c>
@@ -15780,7 +15778,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="60" spans="1:26" hidden="1">
+    <row r="60" spans="1:26">
       <c r="A60" s="66">
         <v>143</v>
       </c>
@@ -15860,7 +15858,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="61" spans="1:26" hidden="1">
+    <row r="61" spans="1:26">
       <c r="A61" s="66">
         <v>143</v>
       </c>
@@ -16101,15 +16099,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA63" xr:uid="{99DC351C-1DDD-4D32-8A0C-932087026D94}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="139"/>
-        <filter val="144"/>
-        <filter val="145"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16120,7 +16109,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -20642,7 +20631,6 @@
       <c r="B1000" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G27" xr:uid="{EBF34D67-BC7B-4C64-B16A-AC837BE8DC25}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -20652,9 +20640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D188" sqref="D188"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -26834,7 +26822,6 @@
       <c r="AC190" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC190" xr:uid="{0FFD6F33-F3F6-4B75-BBF7-D048B5496694}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>